<commit_message>
add first health component, implement it for enemy
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC8016F-C50A-4041-9CCB-0777F3A18D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9DA58E-B730-4864-95E3-24B8225E869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,6 @@
     <t>initial commit, with adding basic mesh model from blender and camera</t>
   </si>
   <si>
-    <t>migrate logs to xls, add upgrade todo's</t>
-  </si>
-  <si>
     <t>apply addon with prototype textures for testmap, add new TODO's + ui prototype</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>What was done :D</t>
+  </si>
+  <si>
+    <t>migrate logs to xls, add upgrade todo's, add spagetti health_component - same for enemy and player, enemy can be damaged by amount of projectile</t>
   </si>
 </sst>
 </file>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1119,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,10 +1131,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1165,7 +1165,7 @@
         <v>45420</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1178,7 +1178,7 @@
         <v>45422</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>45423</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>45424</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1212,7 +1212,7 @@
         <v>45427</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
         <v>45429</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1233,7 +1233,7 @@
         <v>45430</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1241,7 +1241,7 @@
         <v>45431</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>45440</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>45441</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add translations core, damageFlashComponent, particles of shot
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9DA58E-B730-4864-95E3-24B8225E869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C4CA9D-5D00-4B45-A333-6DED29555532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -236,6 +236,21 @@
   </si>
   <si>
     <t>migrate logs to xls, add upgrade todo's, add spagetti health_component - same for enemy and player, enemy can be damaged by amount of projectile</t>
+  </si>
+  <si>
+    <t>in-progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on particles for projectiles - looks good but need finilize for simple attack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on partickles, explosion particles, animation of damage for player and enemies, add lighthing, shaders and fog </t>
+  </si>
+  <si>
+    <t>start work on damage flash component</t>
+  </si>
+  <si>
+    <t>Implement damage flash component - for enemies and player, improve it</t>
   </si>
 </sst>
 </file>
@@ -581,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1119,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1298,6 +1313,38 @@
       </c>
       <c r="B27" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>45445</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>45451</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>45452</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>45455</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
some translation for spark, controller and skill resources system created
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C4CA9D-5D00-4B45-A333-6DED29555532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA9678-6D4B-462E-AFDB-DC5DDAE239DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -250,7 +250,10 @@
     <t>start work on damage flash component</t>
   </si>
   <si>
-    <t>Implement damage flash component - for enemies and player, improve it</t>
+    <t>Implement damage flash component - for enemies and player, improve it. BIG DAY, finally undestand why shooting was bad near walls (cause I calculate direction from weapon to mouse( and they was in one flat axis)), try on first translation staff, start refactoring skills for player - create firs resources</t>
+  </si>
+  <si>
+    <t>add some translation and test it using spark skill resource, add controller system for skill usage by player based on skill_resource + skill_controller + player_skill_controller, with calls using abstact level. Player will be able first to choose which skill he want to use.</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,12 +1342,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45455</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>45456</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add abstraction for controllers and hp/mp/xp layers, add mana regen
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA9678-6D4B-462E-AFDB-DC5DDAE239DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5432B810-8ED2-401B-AB9B-02D1A080845A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -254,6 +254,24 @@
   </si>
   <si>
     <t>add some translation and test it using spark skill resource, add controller system for skill usage by player based on skill_resource + skill_controller + player_skill_controller, with calls using abstact level. Player will be able first to choose which skill he want to use.</t>
+  </si>
+  <si>
+    <t>add abstraction for mana component and etc. found issue that controllets not use the timers of parent</t>
+  </si>
+  <si>
+    <t>Fix issue - not enough to extend script in code, the child component must inherit from parent scene all timers and etc. Implement primitive mana regen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add multilang </t>
+  </si>
+  <si>
+    <t xml:space="preserve">done </t>
+  </si>
+  <si>
+    <t>translate all content before release of demo!</t>
+  </si>
+  <si>
+    <t>UA, ENG, LT</t>
   </si>
 </sst>
 </file>
@@ -297,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -317,6 +335,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +726,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -771,7 +790,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
@@ -797,7 +816,9 @@
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
         <v>24</v>
@@ -810,7 +831,9 @@
       <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -832,8 +855,12 @@
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45455</v>
+      </c>
       <c r="E17" t="s">
         <v>27</v>
       </c>
@@ -947,6 +974,34 @@
       <c r="D26" s="2"/>
       <c r="E26" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="7">
+        <v>45456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -959,7 +1014,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,13 +1413,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>45458</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>45459</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add abstract layersof compoents, refactoring, add glow, polish particles, change resolution
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5432B810-8ED2-401B-AB9B-02D1A080845A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78889856-DBC5-4665-B85E-5EE0C0BBAFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -61,9 +61,6 @@
     <t>improve enemy chasing the player with some pathfinding system</t>
   </si>
   <si>
-    <t>enrich enemies and character with basic HP, MP etc</t>
-  </si>
-  <si>
     <t>todo</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>add first simple light-impulse shot attack with mp usage and some cast time</t>
-  </si>
-  <si>
-    <t>create enemy mp, hp, xp system</t>
   </si>
   <si>
     <t xml:space="preserve"> (if enemy shoot player or hit / kill successfully - he gain exp (next generated enemies of this type and current 1 enemy will be harder + hp, + speed, + dmg)</t>
@@ -272,6 +266,21 @@
   </si>
   <si>
     <t>UA, ENG, LT</t>
+  </si>
+  <si>
+    <t>create enemy mp, hp, xp system AND STAMINA</t>
+  </si>
+  <si>
+    <t>enrich enemies and character with basic HP, MP AND STAMINA</t>
+  </si>
+  <si>
+    <t>Add stamina component, fix inheritence for health and mana components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move player skills to controllers (including jump, run, aim etc.) </t>
+  </si>
+  <si>
+    <t>refactor again - basic stamina and jump controllers used from userSkillController now, fix bugs when skill consume stamina continuasly, add lock system for mana and stamina skills - to avoid paralel skill usages</t>
   </si>
 </sst>
 </file>
@@ -618,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,19 +642,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -723,10 +732,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -735,7 +744,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -749,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
@@ -763,10 +772,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -775,10 +784,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -787,14 +796,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -802,10 +811,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -814,14 +823,14 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -829,10 +838,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -841,10 +850,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -853,7 +862,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
@@ -862,7 +871,7 @@
         <v>45455</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -870,10 +879,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2"/>
     </row>
@@ -882,10 +891,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2"/>
     </row>
@@ -894,10 +903,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -906,10 +915,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -918,10 +927,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -930,10 +939,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -942,10 +951,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -954,10 +963,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -966,14 +975,14 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -981,10 +990,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D27" s="7">
         <v>45456</v>
@@ -995,13 +1004,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1026,19 +1035,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1046,13 +1055,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1060,13 +1069,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1074,13 +1083,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1088,13 +1097,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
@@ -1102,13 +1111,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1116,10 +1125,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -1128,10 +1137,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1140,10 +1149,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -1152,10 +1161,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -1192,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,10 +1213,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1215,7 +1224,7 @@
         <v>45416</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1238,7 +1247,7 @@
         <v>45420</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1251,7 +1260,7 @@
         <v>45422</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1259,7 +1268,7 @@
         <v>45423</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1267,7 +1276,7 @@
         <v>45424</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1285,7 +1294,7 @@
         <v>45427</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1298,7 +1307,7 @@
         <v>45429</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1306,7 +1315,7 @@
         <v>45430</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1314,7 +1323,7 @@
         <v>45431</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1371,7 @@
         <v>45440</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1370,7 +1379,7 @@
         <v>45441</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1378,7 +1387,7 @@
         <v>45445</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1386,7 +1395,7 @@
         <v>45451</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1394,7 +1403,7 @@
         <v>45452</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1402,7 +1411,7 @@
         <v>45455</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1410,7 +1419,7 @@
         <v>45456</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1418,7 +1427,7 @@
         <v>45458</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1426,7 +1435,31 @@
         <v>45459</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>45460</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>45462</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>45463</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add souls structure, animation and etc
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78889856-DBC5-4665-B85E-5EE0C0BBAFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFAE6C5-B0E1-4689-B0C3-E007579DE8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -281,6 +281,12 @@
   </si>
   <si>
     <t>refactor again - basic stamina and jump controllers used from userSkillController now, fix bugs when skill consume stamina continuasly, add lock system for mana and stamina skills - to avoid paralel skill usages</t>
+  </si>
+  <si>
+    <t>work on glow effect (looks nice), fix lags when full screeen - resolution wsa to high - found place where it can be changed, healing animation</t>
+  </si>
+  <si>
+    <t>add souls, souls drop and collecting. Lot of fun, but source consumable… Now enemy on death drop souls, and player can collect them</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,9 +741,11 @@
         <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45466</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -787,9 +795,11 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45466</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1201,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,6 +1470,22 @@
       </c>
       <c r="B37" s="1" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>45465</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>45467</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
pick up souls animation and counting
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFAE6C5-B0E1-4689-B0C3-E007579DE8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D4639-0B93-4EC9-B6E7-861BC24CF8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
     <t>work on glow effect (looks nice), fix lags when full screeen - resolution wsa to high - found place where it can be changed, healing animation</t>
   </si>
   <si>
-    <t>add souls, souls drop and collecting. Lot of fun, but source consumable… Now enemy on death drop souls, and player can collect them</t>
+    <t>add souls, souls drop and collecting. Lot of fun, but source consumable… Now enemy on death drop souls, and player can collect them. Add collecting fade out and counting.</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1480,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>45467</v>
       </c>

</xml_diff>

<commit_message>
souls collecting, enemy components refactor, exp system for player skills and enemies
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D4639-0B93-4EC9-B6E7-861BC24CF8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E696160E-A1D4-40AA-9591-4C19A9F6AF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Version history" sheetId="4" r:id="rId4"/>
     <sheet name="Drawings" sheetId="5" r:id="rId5"/>
     <sheet name="Details" sheetId="6" r:id="rId6"/>
+    <sheet name="insane calcs" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -80,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve"> add enemy hp bar and ? Mp</t>
-  </si>
-  <si>
-    <t>player and ? trap attacks reduce enemy hp (hp shown)</t>
   </si>
   <si>
     <t>add vignette - for fast movement, low hp</t>
@@ -287,6 +285,42 @@
   </si>
   <si>
     <t>add souls, souls drop and collecting. Lot of fun, but source consumable… Now enemy on death drop souls, and player can collect them. Add collecting fade out and counting.</t>
+  </si>
+  <si>
+    <t>refactor enemy, not best but moved almost all to dodge, idle, etc components/controllers</t>
+  </si>
+  <si>
+    <t>finish refactoring enemy, fix bug when player shoot underground while camera close to wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enemy spawner in some rooms </t>
+  </si>
+  <si>
+    <t>close the door - need to kill him - he is static, and spawn enemies</t>
+  </si>
+  <si>
+    <t>add enemy exp system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when enemy does damage to player - it gain exp to enemy exp (all next enemies will be harder and harder) </t>
+  </si>
+  <si>
+    <t>enemy lvl</t>
+  </si>
+  <si>
+    <t>max exp</t>
+  </si>
+  <si>
+    <t>max_lvl</t>
+  </si>
+  <si>
+    <t>add player exp system</t>
+  </si>
+  <si>
+    <t>skills gain exp not player</t>
+  </si>
+  <si>
+    <t>player attacks reduce enemy hp (hp shown)</t>
   </si>
 </sst>
 </file>
@@ -341,9 +375,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -351,6 +382,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,6 +400,1004 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insane calcs'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>enemy lvl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insane calcs'!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-772C-4212-BF51-224AAFB7C1DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insane calcs'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max exp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insane calcs'!$C$3:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>660</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-772C-4212-BF51-224AAFB7C1DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="484953984"/>
+        <c:axId val="484954464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="484953984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484954464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="484954464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="484953984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11DD611F-3DC9-9C1E-DCA6-681DE848198A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -631,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,20 +1679,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -738,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -806,12 +1838,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45473</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
@@ -821,26 +1855,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>45468</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -848,7 +1884,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -863,7 +1899,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -872,7 +1908,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
@@ -881,7 +1917,7 @@
         <v>45455</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -889,19 +1925,21 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="D18" s="6">
+        <v>45473</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -913,7 +1951,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>6</v>
@@ -925,7 +1963,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>6</v>
@@ -937,7 +1975,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
@@ -949,7 +1987,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
@@ -961,7 +1999,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -973,7 +2011,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -985,14 +2023,14 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1000,12 +2038,12 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>45456</v>
       </c>
     </row>
@@ -1014,13 +2052,61 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6">
+        <v>45473</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6">
+        <v>45473</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1044,20 +2130,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1065,13 +2151,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1079,13 +2165,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1093,13 +2179,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1107,13 +2193,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
@@ -1121,13 +2207,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1135,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -1147,7 +2233,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -1159,7 +2245,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -1171,7 +2257,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -1211,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1222,11 +2308,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1234,7 +2320,7 @@
         <v>45416</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1257,7 +2343,7 @@
         <v>45420</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1270,7 +2356,7 @@
         <v>45422</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1278,7 +2364,7 @@
         <v>45423</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1286,7 +2372,7 @@
         <v>45424</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1304,7 +2390,7 @@
         <v>45427</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1317,7 +2403,7 @@
         <v>45429</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1325,7 +2411,7 @@
         <v>45430</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1333,7 +2419,7 @@
         <v>45431</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1381,7 +2467,7 @@
         <v>45440</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1389,7 +2475,7 @@
         <v>45441</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1397,7 +2483,7 @@
         <v>45445</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1405,7 +2491,7 @@
         <v>45451</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1413,7 +2499,7 @@
         <v>45452</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1421,7 +2507,7 @@
         <v>45455</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1429,7 +2515,7 @@
         <v>45456</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1437,7 +2523,7 @@
         <v>45458</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1445,7 +2531,7 @@
         <v>45459</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1453,7 +2539,7 @@
         <v>45460</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1461,7 +2547,7 @@
         <v>45462</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1469,7 +2555,7 @@
         <v>45463</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1477,7 +2563,7 @@
         <v>45465</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1485,11 +2571,24 @@
         <v>45467</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>45468</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>45473</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
@@ -1536,4 +2635,136 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92130128-B324-4549-A9C2-141C6ADD55A7}">
+  <dimension ref="A2:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>C3+($A$3 *B4)+ $A$3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C13" si="0">C4+($A$3 *B5)+ $A$3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add stats bars for enemies and connect them to components
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E696160E-A1D4-40AA-9591-4C19A9F6AF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A49FD-B084-475D-BE63-34A9B12C6BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -290,9 +290,6 @@
     <t>refactor enemy, not best but moved almost all to dodge, idle, etc components/controllers</t>
   </si>
   <si>
-    <t>finish refactoring enemy, fix bug when player shoot underground while camera close to wall</t>
-  </si>
-  <si>
     <t xml:space="preserve">enemy spawner in some rooms </t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>player attacks reduce enemy hp (hp shown)</t>
+  </si>
+  <si>
+    <t>finish refactoring enemy, fix bug when player shoot underground while camera close to wall, add stat bars for enemies</t>
   </si>
 </sst>
 </file>
@@ -1665,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,9 +1899,11 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>45473</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1925,10 +1927,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D18" s="6">
         <v>45473</v>
@@ -2066,13 +2068,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2080,7 +2082,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
@@ -2089,7 +2091,7 @@
         <v>45473</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2097,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
@@ -2106,7 +2108,7 @@
         <v>45473</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2297,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2587,7 +2589,7 @@
         <v>45473</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2653,13 +2655,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add push effect skill and for projectile, fix bugs with camera and enemies
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A49FD-B084-475D-BE63-34A9B12C6BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C2221-8D41-429C-966F-0ECF8BCA5B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>finish refactoring enemy, fix bug when player shoot underground while camera close to wall, add stat bars for enemies</t>
+  </si>
+  <si>
+    <t>finish with mp bar, remove shadows from particles, adjust bars, found prop to glow (hdr2d in subView) - looks ugly), add enemy-spawner for enemies, add vignete on damage, run aim effects</t>
+  </si>
+  <si>
+    <t>fix bug with camera jumps when sprint and aim, fix bug no damage when on head of enemy, add push effect and skill</t>
   </si>
 </sst>
 </file>
@@ -1665,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1812,42 +1818,44 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="3">
-        <v>45466</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D11" s="6">
+        <v>45473</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="6">
-        <v>45473</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>11</v>
+      <c r="D12" s="7">
+        <v>45468</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1855,13 +1863,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="7">
-        <v>45468</v>
+      <c r="D13" s="6">
+        <v>45473</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1869,14 +1877,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45455</v>
+      </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1884,25 +1894,27 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>45473</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D16" s="6">
-        <v>45473</v>
+        <v>45456</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1910,16 +1922,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="3">
-        <v>45455</v>
+      <c r="D17" s="6">
+        <v>45473</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1927,69 +1939,78 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D18" s="6">
         <v>45473</v>
       </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45475</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45475</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45475</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
@@ -1998,10 +2019,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -2010,10 +2031,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -2022,36 +2043,34 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>68</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="6">
-        <v>45456</v>
+        <v>6</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>70</v>
@@ -2068,48 +2087,39 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E29" t="s">
-        <v>81</v>
-      </c>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6">
-        <v>45473</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6">
-        <v>45473</v>
-      </c>
-      <c r="E31" t="s">
-        <v>88</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2121,7 +2131,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2299,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2592,11 +2602,21 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
+    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>45475</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
+      <c r="A43" s="3">
+        <v>45476</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
work on procedural generating of map, get rid of gridmap
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C2221-8D41-429C-966F-0ECF8BCA5B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F8F293-AE45-4FB1-B412-AADC18150A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>fix bug with camera jumps when sprint and aim, fix bug no damage when on head of enemy, add push effect and skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change cursor while casting some skill to some symbols (ua, lt)? </t>
+  </si>
+  <si>
+    <t>oh…a lot of work with light, meshes gridmap, etc., no results only pain and not bad looking some kind of map</t>
+  </si>
+  <si>
+    <t>gridMap removed - shitty staff. Work on random procedure generation of map. Have large progress with common Node3D and script for spawn tiles. Tiles could be spawn as rooms of different sizes, I can spawn long tunels of tiles with almost no collisions(low possibility). Next step apply rooms to tunels and add walls + roof</t>
   </si>
 </sst>
 </file>
@@ -1669,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2120,6 +2129,11 @@
         <v>6</v>
       </c>
       <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2307,10 +2321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2616,6 +2630,22 @@
       </c>
       <c r="B43" s="1" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>45479</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>45480</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random door in random side
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F8F293-AE45-4FB1-B412-AADC18150A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494B414-D7E9-4B59-AFE9-2E838D669314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>gridMap removed - shitty staff. Work on random procedure generation of map. Have large progress with common Node3D and script for spawn tiles. Tiles could be spawn as rooms of different sizes, I can spawn long tunels of tiles with almost no collisions(low possibility). Next step apply rooms to tunels and add walls + roof</t>
+  </si>
+  <si>
+    <t>add generation of exit in random side /random place</t>
   </si>
 </sst>
 </file>
@@ -2321,10 +2324,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2646,6 +2649,14 @@
       </c>
       <c r="B45" s="1" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>45481</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add random generation map (only floor, and corridors) with deadend rooms
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494B414-D7E9-4B59-AFE9-2E838D669314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96BCB25-AFE5-4D4A-9F54-DE85ECE881DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t>add generation of exit in random side /random place</t>
+  </si>
+  <si>
+    <t>fix existing generation of exit. Improve to reduce complexity, first attempts to add additional room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DONE random floor and exist generated perfectly! Next step to clean up that generator class and add the walls </t>
+  </si>
+  <si>
+    <t>Added system of room saving - and now each generated room save some info. Next step to use it while walls generation - to catch where wall should be and where not.</t>
+  </si>
+  <si>
+    <t>Add deadend rooms and modify the common room schema</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2148,7 +2160,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2239,7 +2251,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>37</v>
@@ -2324,10 +2336,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2657,6 +2669,38 @@
       </c>
       <c r="B46" s="1" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>45483</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>45485</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>45492</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>45493</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor mapGenerator, add walls building and clean up code
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96BCB25-AFE5-4D4A-9F54-DE85ECE881DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724D4FA-3B11-4941-9EBE-F5B99FE688AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -350,7 +350,10 @@
     <t>Added system of room saving - and now each generated room save some info. Next step to use it while walls generation - to catch where wall should be and where not.</t>
   </si>
   <si>
-    <t>Add deadend rooms and modify the common room schema</t>
+    <t>Add deadend rooms and modify the common room schema, first attemts to add a walls - not bad  -but lot of work in future</t>
+  </si>
+  <si>
+    <t>Finish walls adding stuff. It works good. Start refactoring the mapGenerator class - extract WallBuilder and SurfaceBuilder</t>
   </si>
 </sst>
 </file>
@@ -2336,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2701,6 +2704,14 @@
       </c>
       <c r="B50" s="1" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>45494</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug with the camera dive into walls
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A724D4FA-3B11-4941-9EBE-F5B99FE688AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E872D08F-4B58-48B7-B014-767740104A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>Finish walls adding stuff. It works good. Start refactoring the mapGenerator class - extract WallBuilder and SurfaceBuilder</t>
+  </si>
+  <si>
+    <t>Fixed the issue when camere went inside the walls - so it was my fail, cause camera shouldn’t be so far from player - if It's - then needed additional configs to handle collisions or etc. cause scene center then can be out of map</t>
   </si>
 </sst>
 </file>
@@ -2339,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2712,6 +2715,14 @@
       </c>
       <c r="B51" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>45495</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor tunel generation of map generator
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E872D08F-4B58-48B7-B014-767740104A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0085C0-634D-4FB4-9C33-83A4CCD0A40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="104">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>Fixed the issue when camere went inside the walls - so it was my fail, cause camera shouldn’t be so far from player - if It's - then needed additional configs to handle collisions or etc. cause scene center then can be out of map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactored tunel generation. Add some  ceil generation. </t>
   </si>
 </sst>
 </file>
@@ -2342,9 +2345,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -2723,6 +2726,14 @@
       </c>
       <c r="B52" s="1" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>45495</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix transparancy of floor and add different heigh ceils
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0085C0-634D-4FB4-9C33-83A4CCD0A40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6571D4F-45EB-436E-BD91-B4395758EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t xml:space="preserve">Refactored tunel generation. Add some  ceil generation. </t>
+  </si>
+  <si>
+    <t>add different heigh room generation, fix floor transparency</t>
   </si>
 </sst>
 </file>
@@ -2345,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2734,6 +2737,14 @@
       </c>
       <c r="B53" s="1" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>45502</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add torch, candle, fix shadows fps drop
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6571D4F-45EB-436E-BD91-B4395758EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F064C028-AA42-4448-9306-A278BB3161E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>add different heigh room generation, fix floor transparency</t>
+  </si>
+  <si>
+    <t>create a torch and candle - add optimisation for shading</t>
   </si>
 </sst>
 </file>
@@ -2348,10 +2351,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,6 +2748,14 @@
       </c>
       <c r="B54" s="1" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>45510</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new models new texutures - work with light and shades, optimisation, generator of torches, of columns
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F064C028-AA42-4448-9306-A278BB3161E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8FAE55-CB99-4BB6-BE87-66A2D5D8A6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -365,7 +365,10 @@
     <t>add different heigh room generation, fix floor transparency</t>
   </si>
   <si>
-    <t>create a torch and candle - add optimisation for shading</t>
+    <t>create a torch and candle - add optimisation for shading, add fog effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work with textures, create new simple meshes in godot for walls, corridors, columns. Debug lights and shadows. </t>
   </si>
 </sst>
 </file>
@@ -2351,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,381 +2384,314 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>45417</v>
+        <v>45420</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>45418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45422</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>45419</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45423</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>45420</v>
+        <v>45424</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>45421</v>
+        <v>45427</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>45422</v>
+        <v>45429</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>45423</v>
+        <v>45430</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>45424</v>
+        <v>45431</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>45425</v>
+        <v>45440</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>45426</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45441</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>45427</v>
+        <v>45445</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>45428</v>
+        <v>45451</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>45429</v>
+        <v>45452</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>45430</v>
+        <v>45455</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>45431</v>
+        <v>45456</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>45432</v>
+        <v>45458</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>45433</v>
+        <v>45459</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>45434</v>
+        <v>45460</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>45435</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45462</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>45436</v>
+        <v>45463</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>45437</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>45465</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>45438</v>
+        <v>45467</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>45439</v>
+      <c r="A25" s="7">
+        <v>45468</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>45440</v>
+        <v>45473</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>45441</v>
+        <v>45475</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>45445</v>
+        <v>45476</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>45451</v>
+        <v>45479</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>45452</v>
+        <v>45480</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>45455</v>
+        <v>45481</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
-        <v>45456</v>
+        <v>45483</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
-        <v>45458</v>
+        <v>45485</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
-        <v>45459</v>
+        <v>45492</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
-        <v>45460</v>
+        <v>45493</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>45462</v>
+        <v>45494</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
-        <v>45463</v>
+        <v>45495</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>45465</v>
+        <v>45495</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
-        <v>45468</v>
+      <c r="A40" s="3">
+        <v>45510</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
-        <v>45473</v>
+        <v>45512</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
-        <v>45475</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
-        <v>45476</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
-        <v>45479</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
-        <v>45480</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
-        <v>45481</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="3">
-        <v>45483</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="3">
-        <v>45485</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="3">
-        <v>45492</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="3">
-        <v>45493</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="3">
-        <v>45494</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
-        <v>45495</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="3">
-        <v>45495</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="3">
-        <v>45502</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
-        <v>45510</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix spawner - spawn batch on player detected
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8FAE55-CB99-4BB6-BE87-66A2D5D8A6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04696C7-2FFA-4FE3-86BD-34AC17A1168F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">work with textures, create new simple meshes in godot for walls, corridors, columns. Debug lights and shadows. </t>
+  </si>
+  <si>
+    <t>add enemies agr each other and fix agr of enemies, looks good</t>
   </si>
 </sst>
 </file>
@@ -2354,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,6 +2695,14 @@
       </c>
       <c r="B41" s="1" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>45532</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add theme, add font, add gui bars, connect bars to player, fix spawner
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04696C7-2FFA-4FE3-86BD-34AC17A1168F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801CF60-9B9D-439C-B2A7-887E16200CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>add enemies agr each other and fix agr of enemies, looks good</t>
+  </si>
+  <si>
+    <t>add mass spawn of enemies on attack or agr zone enter, add primitive player respawn zone and dead souls drop and life minus</t>
+  </si>
+  <si>
+    <t>add gui theme, add custom gui bars, connect them to player, fix spawner</t>
   </si>
 </sst>
 </file>
@@ -2357,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,6 +2709,22 @@
       </c>
       <c r="B42" s="1" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>45539</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>45540</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add radial movement/battle movement of enemies
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801CF60-9B9D-439C-B2A7-887E16200CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D131EC7-6C90-48A8-B2E3-A88ED78223CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -71,9 +71,6 @@
     <t>enemies AI - trying to avoid collision with projectiles</t>
   </si>
   <si>
-    <t>add first stage of game with some aim (requirements in other TODO's)</t>
-  </si>
-  <si>
     <t>add first simple light-impulse shot attack with mp usage and some cast time</t>
   </si>
   <si>
@@ -120,12 +117,6 @@
   </si>
   <si>
     <t>add second stage same but harder</t>
-  </si>
-  <si>
-    <t>add path controll - to open the gate on second shop/stage</t>
-  </si>
-  <si>
-    <t>need to have N energy and souls to open door</t>
   </si>
   <si>
     <t xml:space="preserve"> more mana usage, explode on damage, longer cast time)</t>
@@ -378,6 +369,138 @@
   </si>
   <si>
     <t>add gui theme, add custom gui bars, connect them to player, fix spawner</t>
+  </si>
+  <si>
+    <t>add pickaxe, or skill destructing some blocks</t>
+  </si>
+  <si>
+    <t>add destructive blocks in some room outs</t>
+  </si>
+  <si>
+    <t>using stones you can build the stairs to fontains, and final stairs to next stage</t>
+  </si>
+  <si>
+    <t>add first stage of game with some aim (requirements in other TODO's)( list below)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add path controll - to open the gate on second shop/stage </t>
+  </si>
+  <si>
+    <t>( need to build stairs to next floor)</t>
+  </si>
+  <si>
+    <t>destructive blocks drop stones (even doors)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add collectable gems </t>
+  </si>
+  <si>
+    <t>gems used to activate laser from fontain to door</t>
+  </si>
+  <si>
+    <t>add gold coins</t>
+  </si>
+  <si>
+    <t>used to upgrade character start stats and refil consumable things</t>
+  </si>
+  <si>
+    <t>add consumable tablets (read and drop + consume some souls on usage)</t>
+  </si>
+  <si>
+    <t>after last life lost - all souls lost, and materials - only gold coins left</t>
+  </si>
+  <si>
+    <t>add new enemies (rats or small bugs) - who will spawn all the time</t>
+  </si>
+  <si>
+    <t>add logic that on deadend room spawns the gold, gems and stone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add logic that only after such deadend room will be next fontain and door </t>
+  </si>
+  <si>
+    <t>to be sure - player collect enough gems or can collect to break the door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gold coins could be used to buy the consumable items and upgrade player </t>
+  </si>
+  <si>
+    <t>add enemies movement model when they detect player</t>
+  </si>
+  <si>
+    <t>move readial around player and try to attack spontaniously</t>
+  </si>
+  <si>
+    <t>dead end rooms will contain necessary resources for finishing the stage (gems, gold, stone)</t>
+  </si>
+  <si>
+    <t>destroy door, build stairs</t>
+  </si>
+  <si>
+    <t>add tasks aim of game and replayability, non sleep night gave lot of ideas, hope I will implement them, check additionaly details tab</t>
+  </si>
+  <si>
+    <t>gameplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">before start game player can shop some self upgrades (permanent), and some consumable tablets (hp, mp, stamina, speed up etc.) </t>
+  </si>
+  <si>
+    <t>this updates can be both by only curency which not disapear after death of player - gold, as gold used to be burried with the heroes and etc</t>
+  </si>
+  <si>
+    <t>on menu, before game:</t>
+  </si>
+  <si>
+    <t>game:</t>
+  </si>
+  <si>
+    <t>starts on first room on the fontain, need to reach last room of stage and build stairs to next stage</t>
+  </si>
+  <si>
+    <t>kill enemies gives the souls - main curency during the run, can be spend when use consumable items and to shop between stages - new weapons and consumables</t>
+  </si>
+  <si>
+    <t>stage contain doors which could be oppened using fontain power, to use it player need - collect stones to build stairs to fontain, harwest gems - and put the gems to the fontain fireplace, it will produce shot in the door and door will opened</t>
+  </si>
+  <si>
+    <t>stone, gems and gold could be spawned in common rooms in very low quantities, and in bigger in deadend rooms where will be more enemies</t>
+  </si>
+  <si>
+    <t>game stage will take 1-n doors to open and after last door - need to build the stairs to next floor</t>
+  </si>
+  <si>
+    <t>shop:</t>
+  </si>
+  <si>
+    <t>trader stage - guy who will take souls and will sell you improvements for existing spells or new spells</t>
+  </si>
+  <si>
+    <t>game process:</t>
+  </si>
+  <si>
+    <t>clean up stage, shop, and clean up next stage with harder monsters - as they will be harder after each kick player, or dying.</t>
+  </si>
+  <si>
+    <t>player don’t have own expirience, but have skill expirience system , which will be also saved permanently between stages - so person who bouth n times same weapon and use it - will be more skilled with it</t>
+  </si>
+  <si>
+    <t>game final is to reach ,for instance 5-th floor, after what player can choose to finish story - small text story about that player what happened with player</t>
+  </si>
+  <si>
+    <t>or player can choose to go to endless mode and try to reach as high as possible, score system to compete between players</t>
+  </si>
+  <si>
+    <t>player can die N times and he will throwed back to last fontain, after lives ended - die permanently</t>
+  </si>
+  <si>
+    <t>game could be saved only between stages in the shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learn lowpoly modeling in blender </t>
+  </si>
+  <si>
+    <t>add enemies move randompy circles - looks fine, PI/2 is 90 - it consume one day to debug -_-</t>
   </si>
 </sst>
 </file>
@@ -421,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -442,6 +565,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1720,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1737,19 +1861,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1827,7 +1951,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1869,7 +1993,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -1883,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -1892,7 +2016,7 @@
         <v>45473</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1900,7 +2024,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
@@ -1914,7 +2038,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -1928,7 +2052,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
@@ -1937,7 +2061,7 @@
         <v>45455</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1945,7 +2069,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
@@ -1959,10 +2083,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6">
         <v>45456</v>
@@ -1973,7 +2097,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
@@ -1982,7 +2106,7 @@
         <v>45473</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1990,13 +2114,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" s="6">
         <v>45473</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2004,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
@@ -2018,7 +2142,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>1</v>
@@ -2027,7 +2151,7 @@
         <v>45475</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2035,7 +2159,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>1</v>
@@ -2049,10 +2173,10 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -2061,31 +2185,35 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45520</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45541</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -2097,7 +2225,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -2109,14 +2237,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="2"/>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2124,57 +2251,239 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45541</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45541</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>93</v>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="6">
+        <v>45545</v>
+      </c>
+      <c r="E46" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2187,7 +2496,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2199,19 +2508,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2219,13 +2528,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2233,13 +2542,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2247,13 +2556,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2261,13 +2570,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
@@ -2275,13 +2584,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45536</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2289,7 +2601,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -2301,7 +2613,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2313,7 +2625,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -2325,7 +2637,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -2363,10 +2675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2377,10 +2689,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2388,7 +2700,7 @@
         <v>45416</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2396,7 +2708,7 @@
         <v>45420</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2404,7 +2716,7 @@
         <v>45422</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2412,7 +2724,7 @@
         <v>45423</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2420,7 +2732,7 @@
         <v>45424</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2428,7 +2740,7 @@
         <v>45427</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2436,7 +2748,7 @@
         <v>45429</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2444,7 +2756,7 @@
         <v>45430</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2452,7 +2764,7 @@
         <v>45431</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2460,7 +2772,7 @@
         <v>45440</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2468,7 +2780,7 @@
         <v>45441</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2476,7 +2788,7 @@
         <v>45445</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2484,7 +2796,7 @@
         <v>45451</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2492,7 +2804,7 @@
         <v>45452</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2500,7 +2812,7 @@
         <v>45455</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2508,7 +2820,7 @@
         <v>45456</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2516,7 +2828,7 @@
         <v>45458</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2524,7 +2836,7 @@
         <v>45459</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2532,7 +2844,7 @@
         <v>45460</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2540,7 +2852,7 @@
         <v>45462</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2548,7 +2860,7 @@
         <v>45463</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2556,7 +2868,7 @@
         <v>45465</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2564,7 +2876,7 @@
         <v>45467</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2572,7 +2884,7 @@
         <v>45468</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2580,7 +2892,7 @@
         <v>45473</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2588,7 +2900,7 @@
         <v>45475</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2596,7 +2908,7 @@
         <v>45476</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2604,7 +2916,7 @@
         <v>45479</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2612,7 +2924,7 @@
         <v>45480</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2620,7 +2932,7 @@
         <v>45481</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2628,7 +2940,7 @@
         <v>45483</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2636,7 +2948,7 @@
         <v>45485</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2644,7 +2956,7 @@
         <v>45492</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2652,7 +2964,7 @@
         <v>45493</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2660,7 +2972,7 @@
         <v>45494</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -2668,7 +2980,7 @@
         <v>45495</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2676,7 +2988,7 @@
         <v>45495</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2684,7 +2996,7 @@
         <v>45502</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2692,7 +3004,7 @@
         <v>45510</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2700,7 +3012,7 @@
         <v>45512</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2708,7 +3020,7 @@
         <v>45532</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2716,7 +3028,7 @@
         <v>45539</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2724,7 +3036,31 @@
         <v>45540</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>45543</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>45544</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>45545</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2758,12 +3094,114 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877C5D83-8815-49E8-A7DB-792868407C0A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2784,13 +3222,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add inventory, belt,hands views
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D131EC7-6C90-48A8-B2E3-A88ED78223CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69E9C9-F4E2-4542-AAA1-51B31B4A706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6828" yWindow="2712" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="152">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>add enemies move randompy circles - looks fine, PI/2 is 90 - it consume one day to debug -_-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add belt, inventory, hands views (will change pc - could be long itteruption) </t>
   </si>
 </sst>
 </file>
@@ -1846,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2675,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3061,6 +3064,14 @@
       </c>
       <c r="B47" s="1" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>45548</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
invenory openned by button, ui resizible as well as margins
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69E9C9-F4E2-4542-AAA1-51B31B4A706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C45621F-7626-4940-9C6D-63E154E5B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6828" yWindow="2712" windowWidth="23040" windowHeight="12120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t xml:space="preserve">add belt, inventory, hands views (will change pc - could be long itteruption) </t>
+  </si>
+  <si>
+    <t>add first item to the inventory screen</t>
+  </si>
+  <si>
+    <t>add resizability for the belt, inventory and etc, add button to open/close inventory</t>
   </si>
 </sst>
 </file>
@@ -1853,16 +1859,16 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="66.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1893,7 +1899,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>45427</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>45430</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1991,7 +1997,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2050,7 +2056,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>45456</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2112,7 +2118,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>27</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2171,7 +2177,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2183,7 +2189,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2211,7 +2217,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2223,7 +2229,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2235,7 +2241,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2249,7 +2255,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2291,7 +2297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2346,7 +2352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2357,7 +2363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2404,7 +2410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2415,7 +2421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2472,7 +2478,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2502,14 +2508,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="62.33203125" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="48.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2554,7 +2560,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2582,7 +2588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2611,7 +2617,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2623,7 +2629,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2635,7 +2641,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2647,28 +2653,28 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
     </row>
   </sheetData>
@@ -2678,19 +2684,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="143.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="143.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45416</v>
       </c>
@@ -2706,7 +2712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45420</v>
       </c>
@@ -2714,7 +2720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45422</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>45423</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>45424</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45427</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>45429</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>45430</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>45431</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45440</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45441</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>45445</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>45451</v>
       </c>
@@ -2802,7 +2808,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>45452</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>45455</v>
       </c>
@@ -2818,7 +2824,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45456</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45458</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45459</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45460</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45462</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45463</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>45465</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>45467</v>
       </c>
@@ -2882,7 +2888,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>45468</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>45473</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>45475</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>45476</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>45479</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>45480</v>
       </c>
@@ -2930,7 +2936,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>45481</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>45483</v>
       </c>
@@ -2946,7 +2952,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>45485</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>45492</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>45493</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>45494</v>
       </c>
@@ -2978,7 +2984,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>45495</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>45495</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>45502</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>45510</v>
       </c>
@@ -3010,7 +3016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>45512</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>45532</v>
       </c>
@@ -3026,7 +3032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>45539</v>
       </c>
@@ -3034,7 +3040,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>45540</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>45543</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45544</v>
       </c>
@@ -3058,7 +3064,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45545</v>
       </c>
@@ -3066,12 +3072,28 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>45548</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>45555</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>45556</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3085,7 +3107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3097,7 +3119,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3111,103 +3133,103 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>146</v>
       </c>
@@ -3225,13 +3247,13 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -3242,7 +3264,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -3253,7 +3275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3262,7 +3284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3271,7 +3293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3280,7 +3302,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3289,7 +3311,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3298,7 +3320,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3307,7 +3329,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3316,7 +3338,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3325,7 +3347,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -3334,7 +3356,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
add drag and drop in inventory mode
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C45621F-7626-4940-9C6D-63E154E5B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA8452-7435-4168-B080-2B4F9E0C0AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>add resizability for the belt, inventory and etc, add button to open/close inventory</t>
+  </si>
+  <si>
+    <t>add drag and drop first steps to belt, need to add this for inventory/hands and remove object in old place</t>
+  </si>
+  <si>
+    <t>work on drag and drop</t>
+  </si>
+  <si>
+    <t>work on drag and drop ( I hate this)</t>
+  </si>
+  <si>
+    <t>finally, drag and drop works as I want. Items can be merged or change one anothers place. Player cant drop item or split</t>
   </si>
 </sst>
 </file>
@@ -2684,10 +2696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,6 +3106,38 @@
       </c>
       <c r="B50" s="1" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>45559</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>45562</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>45563</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>45564</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
items connected to skills, can be used in hands, clean up warnings
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA8452-7435-4168-B080-2B4F9E0C0AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDF6179-3958-41A4-907A-6FE4EBA54FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="160">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>finally, drag and drop works as I want. Items can be merged or change one anothers place. Player cant drop item or split</t>
+  </si>
+  <si>
+    <t>items connected to skills, when Item taken to hand - skill can be used!, clean up 50+ warnings</t>
+  </si>
+  <si>
+    <t>final - concept in the phone notes (roof and cubes)</t>
   </si>
 </sst>
 </file>
@@ -1867,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,9 +2203,11 @@
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45562</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2408,7 +2416,10 @@
         <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>6</v>
+        <v>57</v>
+      </c>
+      <c r="D39" s="6">
+        <v>45562</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,7 +2528,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,6 +2677,15 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,10 +2716,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3138,6 +3158,14 @@
       </c>
       <c r="B54" s="1" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>45565</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3287,8 +3315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92130128-B324-4549-A9C2-141C6ADD55A7}">
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
player can collect items and drop to the map
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDF6179-3958-41A4-907A-6FE4EBA54FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8575BB63-2051-4DD0-BCA3-228F672FCA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="166">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -528,6 +528,24 @@
   </si>
   <si>
     <t>final - concept in the phone notes (roof and cubes)</t>
+  </si>
+  <si>
+    <t>should be different and sometimes not collumns but some strange objects</t>
+  </si>
+  <si>
+    <t>Columns randomnless</t>
+  </si>
+  <si>
+    <t>wall color - new levels or rooms should looks different little bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in wall could be traps </t>
+  </si>
+  <si>
+    <t>when player commes to close to wall - wall openes and some enemy shoot player</t>
+  </si>
+  <si>
+    <t>items can be droped and collected to invenory!</t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -2528,7 +2546,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,14 +2706,45 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
@@ -2716,10 +2765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,6 +3215,14 @@
       </c>
       <c r="B55" s="1" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>45566</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3315,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92130128-B324-4549-A9C2-141C6ADD55A7}">
   <dimension ref="A2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add stairs building system for fontains
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46932E6A-5FFE-49BC-B663-363ED9CA5917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44CA0E8-FCD5-4AE5-B796-4EFCB04EADAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="174">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -561,6 +561,18 @@
   </si>
   <si>
     <t>consumable items can be consumed from hands, change controllers and items communicate using items by itself now</t>
+  </si>
+  <si>
+    <t>fix stone drop, add stone gravity, fix enemy spawner</t>
+  </si>
+  <si>
+    <t>start work on stairs to fontain, struggle with tweens</t>
+  </si>
+  <si>
+    <t>add viewport to put items, and spagetti logic to handle hovering and putting items in objects</t>
+  </si>
+  <si>
+    <t>fix fontains, items could be putted and picked by hold action button, can move</t>
   </si>
 </sst>
 </file>
@@ -2792,10 +2804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,6 +3294,38 @@
       </c>
       <c r="B60" s="1" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>45589</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>45602</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>45603</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>45604</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add enemy wall, close path to next room
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4580E3-7F61-46EA-88F8-E4AD495FEA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C8ED4-A76A-4FF9-B544-26DE2F6E1D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>add crystal, crystal controller item/skill, fix fontain</t>
+  </si>
+  <si>
+    <t>start work on new enemy - blocking the entrance between level parts</t>
+  </si>
+  <si>
+    <t>back from depression ;) fix map generation and enemy spawners, separate spawners layer</t>
   </si>
 </sst>
 </file>
@@ -1923,19 +1929,19 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="66.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>45427</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>45430</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2050,7 +2056,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2078,7 +2084,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2168,7 +2174,7 @@
         <v>45456</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>27</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2301,7 +2307,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2313,7 +2319,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2327,7 +2333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2358,7 +2364,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2380,7 +2386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2391,7 +2397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2402,7 +2408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2424,7 +2430,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2474,7 +2480,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2496,7 +2502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2511,7 +2517,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2539,7 +2545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2591,14 +2597,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="62.33203125" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="48.5546875" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2643,7 +2649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2657,7 +2663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2700,7 +2706,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2712,7 +2718,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2724,7 +2730,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2736,7 +2742,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2748,7 +2754,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2774,7 +2780,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2788,16 +2794,16 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
     </row>
   </sheetData>
@@ -2807,19 +2813,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="143.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="143.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -2827,7 +2833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45416</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45420</v>
       </c>
@@ -2843,7 +2849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45422</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>45423</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>45424</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45427</v>
       </c>
@@ -2875,7 +2881,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>45429</v>
       </c>
@@ -2883,7 +2889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>45430</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>45431</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45440</v>
       </c>
@@ -2907,7 +2913,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45441</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>45445</v>
       </c>
@@ -2923,7 +2929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>45451</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>45452</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>45455</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45456</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45458</v>
       </c>
@@ -2963,7 +2969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45459</v>
       </c>
@@ -2971,7 +2977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45460</v>
       </c>
@@ -2979,7 +2985,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45462</v>
       </c>
@@ -2987,7 +2993,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45463</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>45465</v>
       </c>
@@ -3003,7 +3009,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>45467</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>45468</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>45473</v>
       </c>
@@ -3027,7 +3033,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>45475</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>45476</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>45479</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>45480</v>
       </c>
@@ -3059,7 +3065,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>45481</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>45483</v>
       </c>
@@ -3075,7 +3081,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>45485</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>45492</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>45493</v>
       </c>
@@ -3099,7 +3105,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>45494</v>
       </c>
@@ -3107,7 +3113,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>45495</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>45495</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>45502</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>45510</v>
       </c>
@@ -3139,7 +3145,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>45512</v>
       </c>
@@ -3147,7 +3153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>45532</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>45539</v>
       </c>
@@ -3163,7 +3169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>45540</v>
       </c>
@@ -3171,7 +3177,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>45543</v>
       </c>
@@ -3179,7 +3185,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45544</v>
       </c>
@@ -3187,7 +3193,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45545</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>45548</v>
       </c>
@@ -3203,7 +3209,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>45555</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>45556</v>
       </c>
@@ -3219,7 +3225,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>45559</v>
       </c>
@@ -3227,7 +3233,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>45562</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>45563</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>45564</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>45565</v>
       </c>
@@ -3259,7 +3265,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>45575</v>
       </c>
@@ -3267,7 +3273,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>45576</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>45577</v>
       </c>
@@ -3283,7 +3289,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>45582</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>45586</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>45589</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>45602</v>
       </c>
@@ -3315,7 +3321,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>45603</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>45604</v>
       </c>
@@ -3331,12 +3337,28 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>45613</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>45621</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>45632</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3350,7 +3372,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3362,7 +3384,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3376,103 +3398,103 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>146</v>
       </c>
@@ -3490,13 +3512,13 @@
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -3507,7 +3529,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -3518,7 +3540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3527,7 +3549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3536,7 +3558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3545,7 +3567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3554,7 +3576,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3563,7 +3585,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3572,7 +3594,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3581,7 +3603,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3590,7 +3612,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -3599,7 +3621,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
add fireplace collect crystals
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C8ED4-A76A-4FF9-B544-26DE2F6E1D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B7CE8-FFE5-4996-A8B2-C86F12971A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="178">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -582,6 +582,9 @@
   </si>
   <si>
     <t>back from depression ;) fix map generation and enemy spawners, separate spawners layer</t>
+  </si>
+  <si>
+    <t>add fontain fireplace which can collect crystalls</t>
   </si>
 </sst>
 </file>
@@ -2813,10 +2816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,6 +3362,14 @@
       </c>
       <c r="B67" s="1" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>45638</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stone throwing to rigid body
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B7CE8-FFE5-4996-A8B2-C86F12971A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54F07C-C139-4F0E-817E-DBE319992803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="179">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -584,7 +584,10 @@
     <t>back from depression ;) fix map generation and enemy spawners, separate spawners layer</t>
   </si>
   <si>
-    <t>add fontain fireplace which can collect crystalls</t>
+    <t xml:space="preserve">rework stone throwing to rigid body </t>
+  </si>
+  <si>
+    <t>add fontain fireplace which can collect crystalls, and shoot the wall!</t>
   </si>
 </sst>
 </file>
@@ -2816,10 +2819,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3369,6 +3372,14 @@
         <v>45638</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>45639</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rework crystall to rigid body
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54F07C-C139-4F0E-817E-DBE319992803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F687EAC4-D9CA-4C29-B7C4-DB04F9A9737D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -584,10 +584,16 @@
     <t>back from depression ;) fix map generation and enemy spawners, separate spawners layer</t>
   </si>
   <si>
-    <t xml:space="preserve">rework stone throwing to rigid body </t>
-  </si>
-  <si>
     <t>add fontain fireplace which can collect crystalls, and shoot the wall!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rework stone and crystal throwing to rigid body </t>
+  </si>
+  <si>
+    <t>add map to folow player oppened place</t>
+  </si>
+  <si>
+    <t>think to get rid of gold coins concept - better sould to be used</t>
   </si>
 </sst>
 </file>
@@ -1932,10 +1938,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,6 +2586,28 @@
       </c>
       <c r="E46" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2600,13 +2628,14 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="5" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2821,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3372,7 +3401,7 @@
         <v>45638</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3380,7 +3409,7 @@
         <v>45639</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add small animation start for adding souls
</commit_message>
<xml_diff>
--- a/dev_notes.xlsx
+++ b/dev_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F687EAC4-D9CA-4C29-B7C4-DB04F9A9737D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34798E5-F672-416A-914E-4CBBA5E83C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO Before 0.0.1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="183">
   <si>
     <t>create character movement, jumping, dodging</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>think to get rid of gold coins concept - better sould to be used</t>
+  </si>
+  <si>
+    <t>canceled</t>
+  </si>
+  <si>
+    <t>wow what an gap. Long hollidays. Decided to move forward whith what I have to finish project as demo game. Added the souls view and images.</t>
   </si>
 </sst>
 </file>
@@ -1940,20 +1946,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="66.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="66.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>45427</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>45429</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>45430</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>45431</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>45466</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>45468</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2158,7 +2164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>45456</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>27</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>45475</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2279,7 +2285,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2319,7 +2325,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2331,7 +2337,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2376,7 +2382,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2398,7 +2404,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2461,13 +2467,13 @@
         <v>116</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="E37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2475,10 +2481,10 @@
         <v>124</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2492,7 +2498,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
@@ -2607,7 +2613,10 @@
         <v>180</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+      <c r="D48" s="6">
+        <v>45673</v>
       </c>
     </row>
   </sheetData>
@@ -2631,15 +2640,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="62.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -2656,7 +2665,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2670,7 +2679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2684,7 +2693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2712,7 +2721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2729,7 +2738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2741,7 +2750,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2753,7 +2762,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2765,7 +2774,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2777,7 +2786,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2789,7 +2798,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2803,7 +2812,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2815,7 +2824,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2829,16 +2838,16 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="1"/>
     </row>
   </sheetData>
@@ -2848,19 +2857,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125C0613-3EF8-4338-A2F5-AC86E8D2EEFE}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="143.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="143.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>45416</v>
       </c>
@@ -2876,7 +2885,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45420</v>
       </c>
@@ -2884,7 +2893,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45422</v>
       </c>
@@ -2892,7 +2901,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>45423</v>
       </c>
@@ -2900,7 +2909,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>45424</v>
       </c>
@@ -2908,7 +2917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>45427</v>
       </c>
@@ -2916,7 +2925,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45429</v>
       </c>
@@ -2924,7 +2933,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>45430</v>
       </c>
@@ -2932,7 +2941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45431</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45440</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>45441</v>
       </c>
@@ -2956,7 +2965,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>45445</v>
       </c>
@@ -2964,7 +2973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45451</v>
       </c>
@@ -2972,7 +2981,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>45452</v>
       </c>
@@ -2980,7 +2989,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>45455</v>
       </c>
@@ -2988,7 +2997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>45456</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>45458</v>
       </c>
@@ -3004,7 +3013,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45459</v>
       </c>
@@ -3012,7 +3021,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45460</v>
       </c>
@@ -3020,7 +3029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45462</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>45463</v>
       </c>
@@ -3036,7 +3045,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>45465</v>
       </c>
@@ -3044,7 +3053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>45467</v>
       </c>
@@ -3052,7 +3061,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>45468</v>
       </c>
@@ -3060,7 +3069,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45473</v>
       </c>
@@ -3068,7 +3077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>45475</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>45476</v>
       </c>
@@ -3084,7 +3093,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45479</v>
       </c>
@@ -3092,7 +3101,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>45480</v>
       </c>
@@ -3100,7 +3109,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45481</v>
       </c>
@@ -3108,7 +3117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>45483</v>
       </c>
@@ -3116,7 +3125,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>45485</v>
       </c>
@@ -3124,7 +3133,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>45492</v>
       </c>
@@ -3132,7 +3141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>45493</v>
       </c>
@@ -3140,7 +3149,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>45494</v>
       </c>
@@ -3148,7 +3157,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>45495</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>45495</v>
       </c>
@@ -3164,7 +3173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>45502</v>
       </c>
@@ -3172,7 +3181,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>45510</v>
       </c>
@@ -3180,7 +3189,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>45512</v>
       </c>
@@ -3188,7 +3197,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>45532</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>45539</v>
       </c>
@@ -3204,7 +3213,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>45540</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>45543</v>
       </c>
@@ -3220,7 +3229,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45544</v>
       </c>
@@ -3228,7 +3237,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45545</v>
       </c>
@@ -3236,7 +3245,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45548</v>
       </c>
@@ -3244,7 +3253,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>45555</v>
       </c>
@@ -3252,7 +3261,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>45556</v>
       </c>
@@ -3260,7 +3269,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>45559</v>
       </c>
@@ -3268,7 +3277,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>45562</v>
       </c>
@@ -3276,7 +3285,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>45563</v>
       </c>
@@ -3284,7 +3293,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>45564</v>
       </c>
@@ -3292,7 +3301,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>45565</v>
       </c>
@@ -3300,7 +3309,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>45575</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>45576</v>
       </c>
@@ -3316,7 +3325,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>45577</v>
       </c>
@@ -3324,7 +3333,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>45582</v>
       </c>
@@ -3332,7 +3341,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>45586</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>45589</v>
       </c>
@@ -3348,7 +3357,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>45602</v>
       </c>
@@ -3356,7 +3365,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>45603</v>
       </c>
@@ -3364,7 +3373,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>45604</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>45613</v>
       </c>
@@ -3380,7 +3389,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>45621</v>
       </c>
@@ -3388,7 +3397,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>45632</v>
       </c>
@@ -3396,7 +3405,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>45638</v>
       </c>
@@ -3404,12 +3413,20 @@
         <v>177</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>45639</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>45673</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3423,7 +3440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3435,7 +3452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3449,103 +3466,103 @@
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>146</v>
       </c>
@@ -3563,13 +3580,13 @@
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -3580,7 +3597,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -3591,7 +3608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3600,7 +3617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3609,7 +3626,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3618,7 +3635,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3627,7 +3644,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3636,7 +3653,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3645,7 +3662,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3654,7 +3671,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3663,7 +3680,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -3672,7 +3689,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>

</xml_diff>